<commit_message>
Minor fixes and code changes.
</commit_message>
<xml_diff>
--- a/LPManagement.UI/UploadedFiles/Book1.xlsx
+++ b/LPManagement.UI/UploadedFiles/Book1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="57">
   <si>
     <t>S.NO</t>
   </si>
@@ -192,6 +192,9 @@
   </si>
   <si>
     <t>hyderabad</t>
+  </si>
+  <si>
+    <t>Utilization</t>
   </si>
 </sst>
 </file>
@@ -236,7 +239,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -248,6 +251,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -531,15 +537,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AK4"/>
+  <dimension ref="A1:AL4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="AL5" sqref="AL5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -608,7 +614,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:37" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:38" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -692,8 +698,11 @@
       </c>
       <c r="AJ2" s="4"/>
       <c r="AK2" s="4"/>
+      <c r="AL2" s="5" t="s">
+        <v>56</v>
+      </c>
     </row>
-    <row r="3" spans="1:37" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:38" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -763,8 +772,11 @@
       <c r="AK3" s="1" t="s">
         <v>47</v>
       </c>
+      <c r="AL3">
+        <v>100</v>
+      </c>
     </row>
-    <row r="4" spans="1:37" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:38" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -834,9 +846,18 @@
       <c r="AK4" s="1" t="s">
         <v>47</v>
       </c>
+      <c r="AL4">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
     <mergeCell ref="AF1:AF2"/>
     <mergeCell ref="AJ1:AJ2"/>
     <mergeCell ref="AK1:AK2"/>
@@ -846,12 +867,6 @@
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="L1:AC1"/>
     <mergeCell ref="AE1:AE2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E4" r:id="rId1" display="mailto:prabur@virtusa.com"/>

</xml_diff>

<commit_message>
Code changes to persist score details
</commit_message>
<xml_diff>
--- a/LPManagement.UI/UploadedFiles/Book1.xlsx
+++ b/LPManagement.UI/UploadedFiles/Book1.xlsx
@@ -191,7 +191,7 @@
     <t>Chennai</t>
   </si>
   <si>
-    <t>hyderabad</t>
+    <t>Hyderabad</t>
   </si>
   <si>
     <t>Utilization</t>
@@ -250,10 +250,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -540,91 +540,91 @@
   <dimension ref="A1:AL4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="AL5" sqref="AL5"/>
+      <selection activeCell="AH3" sqref="AH3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="5" t="s">
         <v>9</v>
       </c>
       <c r="K1" s="1"/>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4"/>
-      <c r="T1" s="4"/>
-      <c r="U1" s="4"/>
-      <c r="V1" s="4"/>
-      <c r="W1" s="4"/>
-      <c r="X1" s="4"/>
-      <c r="Y1" s="4"/>
-      <c r="Z1" s="4"/>
-      <c r="AA1" s="4"/>
-      <c r="AB1" s="4"/>
-      <c r="AC1" s="4"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5"/>
+      <c r="S1" s="5"/>
+      <c r="T1" s="5"/>
+      <c r="U1" s="5"/>
+      <c r="V1" s="5"/>
+      <c r="W1" s="5"/>
+      <c r="X1" s="5"/>
+      <c r="Y1" s="5"/>
+      <c r="Z1" s="5"/>
+      <c r="AA1" s="5"/>
+      <c r="AB1" s="5"/>
+      <c r="AC1" s="5"/>
       <c r="AD1" s="1"/>
-      <c r="AE1" s="4" t="s">
+      <c r="AE1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="AF1" s="4" t="s">
+      <c r="AF1" s="5" t="s">
         <v>12</v>
       </c>
       <c r="AG1" s="1"/>
       <c r="AH1" s="1"/>
       <c r="AI1" s="1"/>
-      <c r="AJ1" s="4" t="s">
+      <c r="AJ1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="AK1" s="4" t="s">
+      <c r="AK1" s="5" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:38" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
       <c r="K2" s="1" t="s">
         <v>15</v>
       </c>
@@ -685,8 +685,8 @@
       <c r="AD2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AE2" s="4"/>
-      <c r="AF2" s="4"/>
+      <c r="AE2" s="5"/>
+      <c r="AF2" s="5"/>
       <c r="AG2" s="1" t="s">
         <v>35</v>
       </c>
@@ -696,9 +696,9 @@
       <c r="AI2" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AJ2" s="4"/>
-      <c r="AK2" s="4"/>
-      <c r="AL2" s="5" t="s">
+      <c r="AJ2" s="5"/>
+      <c r="AK2" s="5"/>
+      <c r="AL2" s="4" t="s">
         <v>56</v>
       </c>
     </row>
@@ -736,25 +736,63 @@
       <c r="K3" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="1"/>
-      <c r="R3" s="1"/>
-      <c r="S3" s="1"/>
-      <c r="T3" s="1"/>
-      <c r="U3" s="1"/>
-      <c r="V3" s="1"/>
-      <c r="W3" s="1"/>
-      <c r="X3" s="1"/>
-      <c r="Y3" s="1"/>
-      <c r="Z3" s="1"/>
-      <c r="AA3" s="1"/>
-      <c r="AB3" s="1"/>
-      <c r="AC3" s="1"/>
-      <c r="AD3" s="1"/>
+      <c r="L3" s="1">
+        <v>70</v>
+      </c>
+      <c r="M3" s="1">
+        <v>60</v>
+      </c>
+      <c r="N3" s="1">
+        <v>60</v>
+      </c>
+      <c r="O3" s="1">
+        <v>90</v>
+      </c>
+      <c r="P3" s="1">
+        <v>70</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>70</v>
+      </c>
+      <c r="R3" s="1">
+        <v>70</v>
+      </c>
+      <c r="S3" s="1">
+        <v>70</v>
+      </c>
+      <c r="T3" s="1">
+        <v>60</v>
+      </c>
+      <c r="U3" s="1">
+        <v>60</v>
+      </c>
+      <c r="V3" s="1">
+        <v>70</v>
+      </c>
+      <c r="W3" s="1">
+        <v>65</v>
+      </c>
+      <c r="X3" s="1">
+        <v>55</v>
+      </c>
+      <c r="Y3" s="1">
+        <v>55</v>
+      </c>
+      <c r="Z3" s="1">
+        <v>50</v>
+      </c>
+      <c r="AA3" s="1">
+        <v>50</v>
+      </c>
+      <c r="AB3" s="1">
+        <v>90</v>
+      </c>
+      <c r="AC3" s="1">
+        <v>70</v>
+      </c>
+      <c r="AD3" s="1">
+        <v>70</v>
+      </c>
       <c r="AE3" s="1">
         <v>78</v>
       </c>
@@ -771,9 +809,6 @@
       </c>
       <c r="AK3" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="AL3">
-        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:38" ht="60" x14ac:dyDescent="0.25">
@@ -846,18 +881,9 @@
       <c r="AK4" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AL4">
-        <v>0</v>
-      </c>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
     <mergeCell ref="AF1:AF2"/>
     <mergeCell ref="AJ1:AJ2"/>
     <mergeCell ref="AK1:AK2"/>
@@ -867,6 +893,12 @@
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="L1:AC1"/>
     <mergeCell ref="AE1:AE2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E4" r:id="rId1" display="mailto:prabur@virtusa.com"/>

</xml_diff>